<commit_message>
Implemented parallel bayesian with processor limits
</commit_message>
<xml_diff>
--- a/BayesianResults/PriorsTable1.xlsx
+++ b/BayesianResults/PriorsTable1.xlsx
@@ -597,7 +597,7 @@
   <dimension ref="A1:F67"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="G45" sqref="G45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -642,7 +642,7 @@
         <v>0.05</v>
       </c>
       <c r="F2">
-        <v>0.5</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -662,7 +662,7 @@
         <v>0.05</v>
       </c>
       <c r="F3">
-        <v>0.5</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -682,7 +682,7 @@
         <v>0.05</v>
       </c>
       <c r="F4">
-        <v>0.5</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -702,7 +702,7 @@
         <v>0.05</v>
       </c>
       <c r="F5">
-        <v>0.5</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -722,7 +722,7 @@
         <v>0.05</v>
       </c>
       <c r="F6">
-        <v>0.5</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -742,7 +742,7 @@
         <v>0.05</v>
       </c>
       <c r="F7">
-        <v>0.5</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -762,7 +762,7 @@
         <v>0.05</v>
       </c>
       <c r="F8">
-        <v>0.5</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -782,7 +782,7 @@
         <v>0.05</v>
       </c>
       <c r="F9">
-        <v>0.5</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -802,7 +802,7 @@
         <v>0.05</v>
       </c>
       <c r="F10">
-        <v>0.5</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -822,7 +822,7 @@
         <v>0.05</v>
       </c>
       <c r="F11">
-        <v>0.5</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -842,7 +842,7 @@
         <v>0.05</v>
       </c>
       <c r="F12">
-        <v>0.5</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -862,7 +862,7 @@
         <v>0.05</v>
       </c>
       <c r="F13">
-        <v>0.5</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -882,7 +882,7 @@
         <v>0.05</v>
       </c>
       <c r="F14">
-        <v>0.5</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -902,7 +902,7 @@
         <v>0.05</v>
       </c>
       <c r="F15">
-        <v>0.5</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -922,7 +922,7 @@
         <v>0.05</v>
       </c>
       <c r="F16">
-        <v>0.5</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -942,7 +942,7 @@
         <v>0.05</v>
       </c>
       <c r="F17">
-        <v>0.5</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -962,7 +962,7 @@
         <v>0.05</v>
       </c>
       <c r="F18">
-        <v>0.5</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -982,7 +982,7 @@
         <v>0.05</v>
       </c>
       <c r="F19">
-        <v>0.5</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -1002,7 +1002,7 @@
         <v>0.05</v>
       </c>
       <c r="F20">
-        <v>0.5</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -1022,7 +1022,7 @@
         <v>0.05</v>
       </c>
       <c r="F21">
-        <v>0.5</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -1042,7 +1042,7 @@
         <v>0.05</v>
       </c>
       <c r="F22">
-        <v>0.5</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -1062,7 +1062,7 @@
         <v>0.05</v>
       </c>
       <c r="F23">
-        <v>0.5</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -1082,7 +1082,7 @@
         <v>0.05</v>
       </c>
       <c r="F24">
-        <v>0.5</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -1102,7 +1102,7 @@
         <v>0.05</v>
       </c>
       <c r="F25">
-        <v>0.5</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -1122,7 +1122,7 @@
         <v>0.05</v>
       </c>
       <c r="F26">
-        <v>0.5</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -1142,7 +1142,7 @@
         <v>0.05</v>
       </c>
       <c r="F27">
-        <v>0.5</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -1162,7 +1162,7 @@
         <v>0.05</v>
       </c>
       <c r="F28">
-        <v>0.5</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -1182,7 +1182,7 @@
         <v>0.05</v>
       </c>
       <c r="F29">
-        <v>0.5</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -1202,7 +1202,7 @@
         <v>0.05</v>
       </c>
       <c r="F30">
-        <v>0.5</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -1222,7 +1222,7 @@
         <v>0.05</v>
       </c>
       <c r="F31">
-        <v>0.5</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -1242,7 +1242,7 @@
         <v>0.05</v>
       </c>
       <c r="F32">
-        <v>0.5</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -1262,7 +1262,7 @@
         <v>0.05</v>
       </c>
       <c r="F33">
-        <v>0.5</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -1282,7 +1282,7 @@
         <v>0.05</v>
       </c>
       <c r="F34">
-        <v>0.5</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -1302,7 +1302,7 @@
         <v>0.05</v>
       </c>
       <c r="F35">
-        <v>0.5</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -1322,7 +1322,7 @@
         <v>0.05</v>
       </c>
       <c r="F36">
-        <v>0.5</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -1342,7 +1342,7 @@
         <v>0.05</v>
       </c>
       <c r="F37">
-        <v>0.5</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -1362,7 +1362,7 @@
         <v>0.05</v>
       </c>
       <c r="F38">
-        <v>0.5</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -1382,7 +1382,7 @@
         <v>0.05</v>
       </c>
       <c r="F39">
-        <v>0.5</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -1402,7 +1402,7 @@
         <v>0.05</v>
       </c>
       <c r="F40">
-        <v>0.5</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -1422,7 +1422,7 @@
         <v>0.05</v>
       </c>
       <c r="F41">
-        <v>0.5</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -1442,7 +1442,7 @@
         <v>0.05</v>
       </c>
       <c r="F42">
-        <v>0.5</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -1462,7 +1462,7 @@
         <v>0.05</v>
       </c>
       <c r="F43">
-        <v>0.5</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -1482,7 +1482,7 @@
         <v>0.05</v>
       </c>
       <c r="F44">
-        <v>0.5</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -1496,7 +1496,7 @@
         <v>1</v>
       </c>
       <c r="E45">
-        <v>1E-3</v>
+        <v>0.05</v>
       </c>
       <c r="F45">
         <v>0.5</v>
@@ -1513,7 +1513,7 @@
         <v>1</v>
       </c>
       <c r="E46">
-        <v>1E-3</v>
+        <v>0.05</v>
       </c>
       <c r="F46">
         <v>0.5</v>
@@ -1530,7 +1530,7 @@
         <v>1</v>
       </c>
       <c r="E47">
-        <v>1E-3</v>
+        <v>0.05</v>
       </c>
       <c r="F47">
         <v>0.5</v>
@@ -1547,7 +1547,7 @@
         <v>1</v>
       </c>
       <c r="E48">
-        <v>1E-3</v>
+        <v>0.05</v>
       </c>
       <c r="F48">
         <v>0.5</v>
@@ -1564,7 +1564,7 @@
         <v>1</v>
       </c>
       <c r="E49">
-        <v>1E-3</v>
+        <v>0.05</v>
       </c>
       <c r="F49">
         <v>0.5</v>
@@ -1581,7 +1581,7 @@
         <v>1</v>
       </c>
       <c r="E50">
-        <v>1E-3</v>
+        <v>0.05</v>
       </c>
       <c r="F50">
         <v>0.5</v>
@@ -1598,7 +1598,7 @@
         <v>1</v>
       </c>
       <c r="E51">
-        <v>1E-3</v>
+        <v>0.05</v>
       </c>
       <c r="F51">
         <v>0.5</v>
@@ -1615,7 +1615,7 @@
         <v>1</v>
       </c>
       <c r="E52">
-        <v>1E-3</v>
+        <v>0.05</v>
       </c>
       <c r="F52">
         <v>0.5</v>
@@ -1632,7 +1632,7 @@
         <v>1</v>
       </c>
       <c r="E53">
-        <v>1E-3</v>
+        <v>0.05</v>
       </c>
       <c r="F53">
         <v>0.5</v>
@@ -1649,7 +1649,7 @@
         <v>1</v>
       </c>
       <c r="E54">
-        <v>1E-3</v>
+        <v>0.05</v>
       </c>
       <c r="F54">
         <v>0.5</v>
@@ -1666,7 +1666,7 @@
         <v>1</v>
       </c>
       <c r="E55">
-        <v>1E-3</v>
+        <v>0.05</v>
       </c>
       <c r="F55">
         <v>0.5</v>
@@ -1683,7 +1683,7 @@
         <v>1</v>
       </c>
       <c r="E56">
-        <v>1E-3</v>
+        <v>0.05</v>
       </c>
       <c r="F56">
         <v>0.5</v>
@@ -1700,7 +1700,7 @@
         <v>1</v>
       </c>
       <c r="E57">
-        <v>1E-3</v>
+        <v>0.05</v>
       </c>
       <c r="F57">
         <v>0.5</v>
@@ -1717,7 +1717,7 @@
         <v>1</v>
       </c>
       <c r="E58">
-        <v>1E-3</v>
+        <v>0.05</v>
       </c>
       <c r="F58">
         <v>0.5</v>
@@ -1734,7 +1734,7 @@
         <v>1</v>
       </c>
       <c r="E59">
-        <v>1E-3</v>
+        <v>0.05</v>
       </c>
       <c r="F59">
         <v>0.5</v>
@@ -1751,7 +1751,7 @@
         <v>1</v>
       </c>
       <c r="E60">
-        <v>1E-3</v>
+        <v>0.05</v>
       </c>
       <c r="F60">
         <v>0.5</v>
@@ -1768,7 +1768,7 @@
         <v>1</v>
       </c>
       <c r="E61">
-        <v>1E-3</v>
+        <v>0.05</v>
       </c>
       <c r="F61">
         <v>0.5</v>
@@ -1785,7 +1785,7 @@
         <v>1</v>
       </c>
       <c r="E62">
-        <v>1E-3</v>
+        <v>0.05</v>
       </c>
       <c r="F62">
         <v>0.5</v>
@@ -1802,7 +1802,7 @@
         <v>1</v>
       </c>
       <c r="E63">
-        <v>1E-3</v>
+        <v>0.05</v>
       </c>
       <c r="F63">
         <v>0.5</v>
@@ -1819,7 +1819,7 @@
         <v>1</v>
       </c>
       <c r="E64">
-        <v>1E-3</v>
+        <v>0.05</v>
       </c>
       <c r="F64">
         <v>0.5</v>
@@ -1836,7 +1836,7 @@
         <v>1</v>
       </c>
       <c r="E65">
-        <v>1E-3</v>
+        <v>0.05</v>
       </c>
       <c r="F65">
         <v>0.5</v>
@@ -1853,7 +1853,7 @@
         <v>1</v>
       </c>
       <c r="E66">
-        <v>1E-3</v>
+        <v>0.05</v>
       </c>
       <c r="F66">
         <v>0.5</v>
@@ -1870,7 +1870,7 @@
         <v>1</v>
       </c>
       <c r="E67">
-        <v>1E-3</v>
+        <v>0.05</v>
       </c>
       <c r="F67">
         <v>0.5</v>

</xml_diff>

<commit_message>
Ran a few tests
</commit_message>
<xml_diff>
--- a/BayesianResults/PriorsTable1.xlsx
+++ b/BayesianResults/PriorsTable1.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="171027" calcMode="manual" calcCompleted="0" calcOnSave="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -597,7 +597,7 @@
   <dimension ref="A1:F67"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G45" sqref="G45"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -639,7 +639,7 @@
         <v>1</v>
       </c>
       <c r="E2">
-        <v>0.05</v>
+        <v>0.15</v>
       </c>
       <c r="F2">
         <v>-1</v>
@@ -659,7 +659,7 @@
         <v>1</v>
       </c>
       <c r="E3">
-        <v>0.05</v>
+        <v>0.15</v>
       </c>
       <c r="F3">
         <v>-1</v>
@@ -679,7 +679,7 @@
         <v>1</v>
       </c>
       <c r="E4">
-        <v>0.05</v>
+        <v>0.15</v>
       </c>
       <c r="F4">
         <v>-1</v>
@@ -699,7 +699,7 @@
         <v>1</v>
       </c>
       <c r="E5">
-        <v>0.05</v>
+        <v>0.15</v>
       </c>
       <c r="F5">
         <v>-1</v>
@@ -719,7 +719,7 @@
         <v>1</v>
       </c>
       <c r="E6">
-        <v>0.05</v>
+        <v>0.15</v>
       </c>
       <c r="F6">
         <v>-1</v>
@@ -739,7 +739,7 @@
         <v>1</v>
       </c>
       <c r="E7">
-        <v>0.05</v>
+        <v>0.15</v>
       </c>
       <c r="F7">
         <v>-1</v>
@@ -759,7 +759,7 @@
         <v>1</v>
       </c>
       <c r="E8">
-        <v>0.05</v>
+        <v>0.15</v>
       </c>
       <c r="F8">
         <v>-1</v>
@@ -779,7 +779,7 @@
         <v>1</v>
       </c>
       <c r="E9">
-        <v>0.05</v>
+        <v>0.15</v>
       </c>
       <c r="F9">
         <v>-1</v>
@@ -799,7 +799,7 @@
         <v>1</v>
       </c>
       <c r="E10">
-        <v>0.05</v>
+        <v>0.15</v>
       </c>
       <c r="F10">
         <v>-1</v>
@@ -819,7 +819,7 @@
         <v>1</v>
       </c>
       <c r="E11">
-        <v>0.05</v>
+        <v>0.15</v>
       </c>
       <c r="F11">
         <v>-1</v>
@@ -839,7 +839,7 @@
         <v>1</v>
       </c>
       <c r="E12">
-        <v>0.05</v>
+        <v>0.15</v>
       </c>
       <c r="F12">
         <v>-1</v>
@@ -859,7 +859,7 @@
         <v>1</v>
       </c>
       <c r="E13">
-        <v>0.05</v>
+        <v>0.15</v>
       </c>
       <c r="F13">
         <v>-1</v>
@@ -879,7 +879,7 @@
         <v>1</v>
       </c>
       <c r="E14">
-        <v>0.05</v>
+        <v>0.15</v>
       </c>
       <c r="F14">
         <v>-1</v>
@@ -899,7 +899,7 @@
         <v>1</v>
       </c>
       <c r="E15">
-        <v>0.05</v>
+        <v>0.15</v>
       </c>
       <c r="F15">
         <v>-1</v>
@@ -919,7 +919,7 @@
         <v>1</v>
       </c>
       <c r="E16">
-        <v>0.05</v>
+        <v>0.15</v>
       </c>
       <c r="F16">
         <v>-1</v>
@@ -939,7 +939,7 @@
         <v>1</v>
       </c>
       <c r="E17">
-        <v>0.05</v>
+        <v>0.15</v>
       </c>
       <c r="F17">
         <v>-1</v>
@@ -959,7 +959,7 @@
         <v>1</v>
       </c>
       <c r="E18">
-        <v>0.05</v>
+        <v>0.15</v>
       </c>
       <c r="F18">
         <v>-1</v>
@@ -979,7 +979,7 @@
         <v>1</v>
       </c>
       <c r="E19">
-        <v>0.05</v>
+        <v>0.15</v>
       </c>
       <c r="F19">
         <v>-1</v>
@@ -999,7 +999,7 @@
         <v>1</v>
       </c>
       <c r="E20">
-        <v>0.05</v>
+        <v>0.15</v>
       </c>
       <c r="F20">
         <v>-1</v>
@@ -1019,7 +1019,7 @@
         <v>1</v>
       </c>
       <c r="E21">
-        <v>0.05</v>
+        <v>0.15</v>
       </c>
       <c r="F21">
         <v>-1</v>
@@ -1039,7 +1039,7 @@
         <v>1</v>
       </c>
       <c r="E22">
-        <v>0.05</v>
+        <v>0.15</v>
       </c>
       <c r="F22">
         <v>-1</v>

</xml_diff>

<commit_message>
Ran Priors with _1
</commit_message>
<xml_diff>
--- a/BayesianResults/PriorsTable1.xlsx
+++ b/BayesianResults/PriorsTable1.xlsx
@@ -1,22 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18229"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="26215"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\SALES\Fundos de Mercado\Pedro Mattos\Notebooks\Nowcasting\BayesianResults\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/PedroBraz2/Documents/Repos/Nowcasting/BayesianResults/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14340" windowHeight="9135"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14240"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027" calcMode="manual" calcCompleted="0" calcOnSave="0"/>
+  <calcPr calcId="150001" calcMode="manual" calcCompleted="0" calcOnSave="0" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -248,11 +251,27 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -275,13 +294,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="7">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -596,19 +627,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F67"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3:E44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -625,7 +656,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -636,16 +667,16 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E2">
-        <v>0.15</v>
+        <v>0.2</v>
       </c>
       <c r="F2">
         <v>-1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -656,16 +687,16 @@
         <v>0</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E3">
-        <v>0.15</v>
+        <v>0.2</v>
       </c>
       <c r="F3">
         <v>-1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -676,16 +707,16 @@
         <v>0</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E4">
-        <v>0.15</v>
+        <v>0.2</v>
       </c>
       <c r="F4">
         <v>-1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -696,16 +727,16 @@
         <v>0</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E5">
-        <v>0.15</v>
+        <v>0.2</v>
       </c>
       <c r="F5">
         <v>-1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -716,16 +747,16 @@
         <v>0</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E6">
-        <v>0.15</v>
+        <v>0.2</v>
       </c>
       <c r="F6">
         <v>-1</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -736,16 +767,16 @@
         <v>0</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E7">
-        <v>0.15</v>
+        <v>0.2</v>
       </c>
       <c r="F7">
         <v>-1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -756,16 +787,16 @@
         <v>0</v>
       </c>
       <c r="D8">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E8">
-        <v>0.15</v>
+        <v>0.2</v>
       </c>
       <c r="F8">
         <v>-1</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -776,16 +807,16 @@
         <v>0</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E9">
-        <v>0.15</v>
+        <v>0.2</v>
       </c>
       <c r="F9">
         <v>-1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -796,16 +827,16 @@
         <v>0</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E10">
-        <v>0.15</v>
+        <v>0.2</v>
       </c>
       <c r="F10">
         <v>-1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -816,16 +847,16 @@
         <v>0</v>
       </c>
       <c r="D11">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E11">
-        <v>0.15</v>
+        <v>0.2</v>
       </c>
       <c r="F11">
         <v>-1</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -836,16 +867,16 @@
         <v>0</v>
       </c>
       <c r="D12">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E12">
-        <v>0.15</v>
+        <v>0.2</v>
       </c>
       <c r="F12">
         <v>-1</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -856,16 +887,16 @@
         <v>0</v>
       </c>
       <c r="D13">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E13">
-        <v>0.15</v>
+        <v>0.2</v>
       </c>
       <c r="F13">
         <v>-1</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -876,16 +907,16 @@
         <v>0</v>
       </c>
       <c r="D14">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E14">
-        <v>0.15</v>
+        <v>0.2</v>
       </c>
       <c r="F14">
         <v>-1</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -896,16 +927,16 @@
         <v>0</v>
       </c>
       <c r="D15">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E15">
-        <v>0.15</v>
+        <v>0.2</v>
       </c>
       <c r="F15">
         <v>-1</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -916,16 +947,16 @@
         <v>0</v>
       </c>
       <c r="D16">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E16">
-        <v>0.15</v>
+        <v>0.2</v>
       </c>
       <c r="F16">
         <v>-1</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -936,16 +967,16 @@
         <v>0</v>
       </c>
       <c r="D17">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E17">
-        <v>0.15</v>
+        <v>0.2</v>
       </c>
       <c r="F17">
         <v>-1</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -956,16 +987,16 @@
         <v>0</v>
       </c>
       <c r="D18">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E18">
-        <v>0.15</v>
+        <v>0.2</v>
       </c>
       <c r="F18">
         <v>-1</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>20</v>
       </c>
@@ -976,16 +1007,16 @@
         <v>0</v>
       </c>
       <c r="D19">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E19">
-        <v>0.15</v>
+        <v>0.2</v>
       </c>
       <c r="F19">
         <v>-1</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -996,16 +1027,16 @@
         <v>0</v>
       </c>
       <c r="D20">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E20">
-        <v>0.15</v>
+        <v>0.2</v>
       </c>
       <c r="F20">
         <v>-1</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -1016,16 +1047,16 @@
         <v>0</v>
       </c>
       <c r="D21">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E21">
-        <v>0.15</v>
+        <v>0.2</v>
       </c>
       <c r="F21">
         <v>-1</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>23</v>
       </c>
@@ -1036,16 +1067,16 @@
         <v>0</v>
       </c>
       <c r="D22">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E22">
-        <v>0.15</v>
+        <v>0.2</v>
       </c>
       <c r="F22">
         <v>-1</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -1056,16 +1087,16 @@
         <v>0</v>
       </c>
       <c r="D23">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E23">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="F23">
         <v>-1</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>25</v>
       </c>
@@ -1076,16 +1107,16 @@
         <v>0</v>
       </c>
       <c r="D24">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E24">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="F24">
         <v>-1</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>26</v>
       </c>
@@ -1096,16 +1127,16 @@
         <v>0</v>
       </c>
       <c r="D25">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E25">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="F25">
         <v>-1</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>27</v>
       </c>
@@ -1116,16 +1147,16 @@
         <v>0</v>
       </c>
       <c r="D26">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E26">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="F26">
         <v>-1</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>28</v>
       </c>
@@ -1136,16 +1167,16 @@
         <v>0</v>
       </c>
       <c r="D27">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E27">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="F27">
         <v>-1</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>29</v>
       </c>
@@ -1156,16 +1187,16 @@
         <v>0</v>
       </c>
       <c r="D28">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E28">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="F28">
         <v>-1</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>30</v>
       </c>
@@ -1176,16 +1207,16 @@
         <v>0</v>
       </c>
       <c r="D29">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E29">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="F29">
         <v>-1</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>31</v>
       </c>
@@ -1196,16 +1227,16 @@
         <v>0</v>
       </c>
       <c r="D30">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E30">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="F30">
         <v>-1</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>32</v>
       </c>
@@ -1216,16 +1247,16 @@
         <v>0</v>
       </c>
       <c r="D31">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E31">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="F31">
         <v>-1</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>33</v>
       </c>
@@ -1236,16 +1267,16 @@
         <v>0</v>
       </c>
       <c r="D32">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E32">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="F32">
         <v>-1</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>34</v>
       </c>
@@ -1256,16 +1287,16 @@
         <v>0</v>
       </c>
       <c r="D33">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E33">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="F33">
         <v>-1</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>35</v>
       </c>
@@ -1276,16 +1307,16 @@
         <v>0</v>
       </c>
       <c r="D34">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E34">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="F34">
         <v>-1</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>36</v>
       </c>
@@ -1296,16 +1327,16 @@
         <v>0</v>
       </c>
       <c r="D35">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E35">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="F35">
         <v>-1</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>37</v>
       </c>
@@ -1316,16 +1347,16 @@
         <v>0</v>
       </c>
       <c r="D36">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E36">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="F36">
         <v>-1</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>38</v>
       </c>
@@ -1336,16 +1367,16 @@
         <v>0</v>
       </c>
       <c r="D37">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E37">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="F37">
         <v>-1</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>39</v>
       </c>
@@ -1356,16 +1387,16 @@
         <v>0</v>
       </c>
       <c r="D38">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E38">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="F38">
         <v>-1</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>40</v>
       </c>
@@ -1376,16 +1407,16 @@
         <v>0</v>
       </c>
       <c r="D39">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E39">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="F39">
         <v>-1</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>41</v>
       </c>
@@ -1396,16 +1427,16 @@
         <v>0</v>
       </c>
       <c r="D40">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E40">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="F40">
         <v>-1</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>42</v>
       </c>
@@ -1416,16 +1447,16 @@
         <v>0</v>
       </c>
       <c r="D41">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E41">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="F41">
         <v>-1</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>43</v>
       </c>
@@ -1436,16 +1467,16 @@
         <v>0</v>
       </c>
       <c r="D42">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E42">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="F42">
         <v>-1</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>44</v>
       </c>
@@ -1456,16 +1487,16 @@
         <v>0</v>
       </c>
       <c r="D43">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E43">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="F43">
         <v>-1</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>45</v>
       </c>
@@ -1476,16 +1507,16 @@
         <v>0</v>
       </c>
       <c r="D44">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E44">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="F44">
         <v>-1</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>46</v>
       </c>
@@ -1502,7 +1533,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>47</v>
       </c>
@@ -1519,7 +1550,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>48</v>
       </c>
@@ -1536,7 +1567,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>49</v>
       </c>
@@ -1553,7 +1584,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>50</v>
       </c>
@@ -1570,7 +1601,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>51</v>
       </c>
@@ -1587,7 +1618,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>52</v>
       </c>
@@ -1604,7 +1635,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>53</v>
       </c>
@@ -1621,7 +1652,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>54</v>
       </c>
@@ -1638,7 +1669,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>55</v>
       </c>
@@ -1655,7 +1686,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>56</v>
       </c>
@@ -1672,7 +1703,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>57</v>
       </c>
@@ -1689,7 +1720,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>58</v>
       </c>
@@ -1706,7 +1737,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>59</v>
       </c>
@@ -1723,7 +1754,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>60</v>
       </c>
@@ -1740,7 +1771,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>61</v>
       </c>
@@ -1757,7 +1788,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>62</v>
       </c>
@@ -1774,7 +1805,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>63</v>
       </c>
@@ -1791,7 +1822,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>64</v>
       </c>
@@ -1808,7 +1839,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>65</v>
       </c>
@@ -1825,7 +1856,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>66</v>
       </c>
@@ -1842,7 +1873,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>67</v>
       </c>
@@ -1859,7 +1890,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>68</v>
       </c>
@@ -1878,5 +1909,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>